<commit_message>
add masking password feature
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91945\eclipse-workspace\SeleniumAutomationFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C5BEC1-31DB-499B-834E-F5CBF39FA221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AED49E-9BCD-410E-8846-922A24DB2B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
   <si>
     <t>Testname</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>amazonTest</t>
+  </si>
+  <si>
+    <t>YWRtaW4xMjM=</t>
   </si>
 </sst>
 </file>
@@ -536,7 +539,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -586,7 +589,7 @@
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -609,7 +612,7 @@
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -692,7 +695,7 @@
         <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>

</xml_diff>